<commit_message>
Better handling of unbounded XLSX for preview
</commit_message>
<xml_diff>
--- a/public/sample_uploads/portfolio_investments_for_as_of_report.xlsx
+++ b/public/sample_uploads/portfolio_investments_for_as_of_report.xlsx
@@ -608,20 +608,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="28.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="10.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="20.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.27"/>
@@ -845,14 +845,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I2:I1005" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="I2:I7" type="list">
       <formula1>"Domestic,Overseas"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>